<commit_message>
Updated team report 06
</commit_message>
<xml_diff>
--- a/Team06Report.xlsx
+++ b/Team06Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="300" windowWidth="20730" windowHeight="11700" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14310" windowHeight="6690" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="220">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>Review each other code</t>
+  </si>
+  <si>
+    <t>Not check in updated gedcom file in github</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9426527196669955E-2"/>
+          <c:y val="7.6557126781105655E-2"/>
+          <c:w val="0.90340386157089791"/>
+          <c:h val="0.82811015433316582"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -985,7 +998,13 @@
                   <c:v>40808</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40820</c:v>
+                  <c:v>40822</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40836</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,6 +1021,12 @@
                 <c:pt idx="1">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1017,11 +1042,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104963072"/>
-        <c:axId val="96498432"/>
+        <c:axId val="74780032"/>
+        <c:axId val="55436416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104963072"/>
+        <c:axId val="74780032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,14 +1056,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96498432"/>
+        <c:crossAx val="55436416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="96498432"/>
+        <c:axId val="55436416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104963072"/>
+        <c:crossAx val="74780032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1541,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D13"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E25" sqref="B20:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1685,6 +1710,9 @@
       <c r="D8" s="14" t="s">
         <v>160</v>
       </c>
+      <c r="E8" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1699,6 +1727,9 @@
       <c r="D9" t="s">
         <v>160</v>
       </c>
+      <c r="E9" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1713,6 +1744,9 @@
       <c r="D10" s="14" t="s">
         <v>164</v>
       </c>
+      <c r="E10" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1727,6 +1761,9 @@
       <c r="D11" s="14" t="s">
         <v>164</v>
       </c>
+      <c r="E11" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1741,6 +1778,9 @@
       <c r="D12" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="E12" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1755,6 +1795,9 @@
       <c r="D13" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="E13" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1769,6 +1812,9 @@
       <c r="D14" t="s">
         <v>160</v>
       </c>
+      <c r="E14" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1783,6 +1829,9 @@
       <c r="D15" t="s">
         <v>160</v>
       </c>
+      <c r="E15" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1797,8 +1846,11 @@
       <c r="D16" s="14" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1811,8 +1863,11 @@
       <c r="D17" s="14" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1825,8 +1880,11 @@
       <c r="D18" s="14" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1839,8 +1897,11 @@
       <c r="D19" s="14" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -1854,7 +1915,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1868,7 +1929,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1882,7 +1943,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1896,7 +1957,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1910,7 +1971,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1941,10 +2002,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1996,7 +2057,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>40820</v>
+        <v>40822</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -2014,6 +2075,48 @@
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
         <v>97.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>40836</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>536</v>
+      </c>
+      <c r="E4">
+        <v>125</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4*60</f>
+        <v>84.47999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>40850</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>711</v>
+      </c>
+      <c r="E5">
+        <v>110</v>
+      </c>
+      <c r="F5" s="9">
+        <f>(D5-D4)/E5*60</f>
+        <v>95.454545454545453</v>
       </c>
     </row>
   </sheetData>
@@ -2033,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A32" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2531,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2540,7 +2643,7 @@
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2569,7 +2672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>137</v>
       </c>
@@ -2579,11 +2682,23 @@
       <c r="C2" s="14" t="s">
         <v>160</v>
       </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
         <v>15</v>
+      </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2596,11 +2711,23 @@
       <c r="C3" t="s">
         <v>160</v>
       </c>
+      <c r="D3" t="s">
+        <v>211</v>
+      </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
         <v>25</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2613,11 +2740,23 @@
       <c r="C4" s="14" t="s">
         <v>164</v>
       </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4">
         <v>10</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2630,11 +2769,23 @@
       <c r="C5" s="14" t="s">
         <v>164</v>
       </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
       <c r="E5">
         <v>20</v>
       </c>
       <c r="F5">
         <v>30</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -2647,11 +2798,23 @@
       <c r="C6" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
         <v>30</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2664,11 +2827,23 @@
       <c r="C7" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="D7" t="s">
+        <v>211</v>
+      </c>
       <c r="E7">
         <v>25</v>
       </c>
       <c r="F7">
         <v>40</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2685,15 +2860,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2721,6 +2899,225 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2735,13 +3132,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="31.125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -2770,6 +3171,108 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>